<commit_message>
Add Iso picture and results - Cifar100 Densenet
</commit_message>
<xml_diff>
--- a/Results Documentation/Image Classification/Cifar100/DenseNet-BC-100/Results Sheet.xlsx
+++ b/Results Documentation/Image Classification/Cifar100/DenseNet-BC-100/Results Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avichai\Desktop\Technion\Project_A\Deep-Neural-Networks-Calibration\Results Documentation\Image Classification\Cifar100\DenseNet-BC-100\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBF8065-8649-4DDE-9195-A91180E53D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19728513-D8BC-4B3F-BB07-75F40712EB0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA86E257-BB19-4E9E-8059-887006D9CF09}"/>
+    <workbookView xWindow="3750" yWindow="1140" windowWidth="21600" windowHeight="11385" xr2:uid="{AA86E257-BB19-4E9E-8059-887006D9CF09}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>Model</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Histogram Bins</t>
+  </si>
+  <si>
+    <t>Isotonic</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -702,7 +705,31 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I8" s="1"/>
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
+        <v>0.74968000000000001</v>
+      </c>
+      <c r="G8" s="2">
+        <v>6.5079999999999999E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>4.7219999999999998E-2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.1356</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I9" s="1"/>

</xml_diff>